<commit_message>
Ajute no formato dos valores de saída das taxas efetivas anuais.
</commit_message>
<xml_diff>
--- a/dados_entrada.xlsx
+++ b/dados_entrada.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\HD-Antigo\Documentos\ProjetosDigitais\Projetos\Python\sim-valor_imovel_e_aluguel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544F06EF-D3E9-4F5A-AB10-15784569123E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B14401-031C-4980-96CB-6342BCBA9832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Entrada da compra" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Aluguel</t>
   </si>
@@ -72,6 +73,30 @@
   </si>
   <si>
     <t>https://www.zapimoveis.com.br/imovel/venda-apartamento-3-quartos-com-piscina-boa-viagem-recife-pe-93m2-id-2710871835/</t>
+  </si>
+  <si>
+    <t>Fonte</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Valor Liquido</t>
+  </si>
+  <si>
+    <t>CDB BANCO MASTER DE INVESTIME - ABR/2030</t>
+  </si>
+  <si>
+    <t>ARX Hedge FIC INFRA RF</t>
+  </si>
+  <si>
+    <t>FGTS</t>
+  </si>
+  <si>
+    <t>Edileuza - Xp CDI Debêntures Incetivadas</t>
+  </si>
+  <si>
+    <t>Edileuza - ARX Hedge FIC INFRA RF</t>
   </si>
 </sst>
 </file>
@@ -81,7 +106,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +131,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,7 +206,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -204,6 +237,12 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hiperlink" xfId="3" builtinId="8"/>
@@ -490,7 +529,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +582,8 @@
         <v>749</v>
       </c>
       <c r="D2" s="3">
-        <v>497968.29</v>
+        <f>'Entrada da compra'!C7</f>
+        <v>504134.27999999997</v>
       </c>
       <c r="E2" s="4">
         <v>0.1099</v>
@@ -593,4 +633,96 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4FAB3CB-2641-4A32-826C-4A716FDF5DA1}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="12">
+        <v>45711</v>
+      </c>
+      <c r="C2" s="13">
+        <v>109833.27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="12">
+        <v>45711</v>
+      </c>
+      <c r="C3" s="13">
+        <v>116234.39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="12">
+        <v>45711</v>
+      </c>
+      <c r="C4" s="13">
+        <v>219442.32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="12">
+        <v>45711</v>
+      </c>
+      <c r="C5" s="13">
+        <v>11532.87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="12">
+        <v>45711</v>
+      </c>
+      <c r="C6" s="13">
+        <v>47091.43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" s="15">
+        <f>SUM(C2:C6)</f>
+        <v>504134.27999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>